<commit_message>
added best tours to the report
</commit_message>
<xml_diff>
--- a/Project4/andrewsAlgo/Example Results.xlsx
+++ b/Project4/andrewsAlgo/Example Results.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -25,19 +25,19 @@
     <t>Time</t>
   </si>
   <si>
-    <t>tsp_example_1.txt</t>
-  </si>
-  <si>
-    <t>tsp_example_2.txt</t>
-  </si>
-  <si>
-    <t>tsp_example_3.txt</t>
+    <t>tsp_example_1.txt.tour</t>
+  </si>
+  <si>
+    <t>tsp_example_2.txt.tour</t>
+  </si>
+  <si>
+    <t>tsp_example_3.txt.tour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -55,7 +55,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -63,12 +63,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,55 +392,56 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>106817</v>
       </c>
-      <c r="C2">
-        <v>8.5000000000000006E-2</v>
+      <c r="C2" s="1">
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>2452</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>2.2799999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>1964948</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>73.198989999999995</v>
       </c>
     </row>

</xml_diff>